<commit_message>
added details about pipeline in result analysis
</commit_message>
<xml_diff>
--- a/results/ResultAnalysis.xlsx
+++ b/results/ResultAnalysis.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vikrambahadur/Library/Mobile Documents/com~apple~CloudDocs/QFM/ML/project/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CA8697E-0F46-C048-B539-66F4C917E2AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBF97513-A6BA-5743-A318-1356FDFD98CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="43480" yWindow="-500" windowWidth="30180" windowHeight="19400" xr2:uid="{066441B5-DF56-C841-B82C-5C53858E106E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="19">
   <si>
     <t>Predicted Label</t>
   </si>
@@ -89,6 +89,16 @@
   </si>
   <si>
     <t>LR (Logistic Regression)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Model is made from Pipeline	
+where Pipeline has ""preprocessor"" and ""model"" in use	
+preprocessor consists -&gt; Columns Transformer made from further pipelines for numeric and categorical features	
+for numeric we have SimpleImputer ( to fill missing values) and StandardScaler (to removes the mean and scales each feature/variable to unit variance)							
+for cateogorical we have OneHotEncoder(integer representation)							
+we split the data with 80% (taining) 20% (testing) and assign to X_train, X_test, y_train, y_test							
+we fit the mode using X_train, y_train and score it using X_test, y_test and finally predit X_test to y_preds							
+To analysis result we use crrostab to create confusion matrix and classification report to get same in report form.								</t>
   </si>
 </sst>
 </file>
@@ -181,7 +191,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
@@ -197,6 +207,9 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -511,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69E7CE99-65C9-E744-B048-AD37273A866D}">
-  <dimension ref="C1:J43"/>
+  <dimension ref="C2:J53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="155" zoomScaleNormal="155" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -523,220 +536,161 @@
     <col min="4" max="5" width="5.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C1" s="1" t="s">
+    <row r="2" spans="3:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C2" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+    </row>
+    <row r="3" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+    </row>
+    <row r="4" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+    </row>
+    <row r="5" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+    </row>
+    <row r="6" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+    </row>
+    <row r="7" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+    </row>
+    <row r="8" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+    </row>
+    <row r="9" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+    </row>
+    <row r="11" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" t="s">
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-    </row>
-    <row r="2" spans="3:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="14">
-        <v>41188</v>
-      </c>
-      <c r="G2" s="1">
-        <v>36548</v>
-      </c>
-      <c r="H2" s="1">
-        <v>4640</v>
-      </c>
-      <c r="I2" s="1">
-        <f>G2+H2</f>
-        <v>41188</v>
-      </c>
-      <c r="J2" s="1"/>
-    </row>
-    <row r="3" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="F3" s="13">
-        <f>F2*0.2</f>
-        <v>8237.6</v>
-      </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-    </row>
-    <row r="4" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="11">
-        <v>0.8</v>
-      </c>
-      <c r="F4" s="1">
-        <f>F2*0.8</f>
-        <v>32950.400000000001</v>
-      </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-    </row>
-    <row r="5" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-    </row>
-    <row r="6" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C6" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-    </row>
-    <row r="7" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C7" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-    </row>
-    <row r="8" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C8" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" s="3">
-        <v>7198</v>
-      </c>
-      <c r="E8" s="3">
-        <v>93</v>
-      </c>
-      <c r="F8" s="1">
-        <f>D8+E8</f>
-        <v>7291</v>
-      </c>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-    </row>
-    <row r="9" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" s="3">
-        <v>706</v>
-      </c>
-      <c r="E9" s="3">
-        <v>241</v>
-      </c>
-      <c r="F9" s="1">
-        <f>D9+E9</f>
-        <v>947</v>
-      </c>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-    </row>
-    <row r="10" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="13">
-        <f>F8+F9</f>
-        <v>8238</v>
-      </c>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-    </row>
-    <row r="11" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C11" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="3:10" ht="19" x14ac:dyDescent="0.25">
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
+      <c r="F12" s="14">
+        <v>41188</v>
+      </c>
+      <c r="G12" s="1">
+        <v>36548</v>
+      </c>
+      <c r="H12" s="1">
+        <v>4640</v>
+      </c>
+      <c r="I12" s="1">
+        <f>G12+H12</f>
+        <v>41188</v>
+      </c>
       <c r="J12" s="1"/>
     </row>
     <row r="13" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C13" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="F13" s="13">
+        <f>F12*0.2</f>
+        <v>8237.6</v>
+      </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
     </row>
     <row r="14" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C14" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="F14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="11">
+        <v>0.8</v>
+      </c>
+      <c r="F14" s="1">
+        <f>F12*0.8</f>
+        <v>32950.400000000001</v>
+      </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
     </row>
     <row r="15" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C15" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
+      <c r="C15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
@@ -744,50 +698,46 @@
       <c r="J15" s="1"/>
     </row>
     <row r="16" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D16" s="5">
-        <v>7204</v>
-      </c>
-      <c r="E16" s="5">
-        <v>106</v>
-      </c>
-      <c r="F16" s="1">
-        <f>D16+E16</f>
-        <v>7310</v>
-      </c>
+      <c r="E16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
     </row>
     <row r="17" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C17" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D17" s="5">
-        <v>726</v>
-      </c>
-      <c r="E17" s="5">
-        <v>202</v>
-      </c>
-      <c r="F17" s="1">
-        <f>D17+E17</f>
-        <v>928</v>
-      </c>
+      <c r="C17" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
     </row>
     <row r="18" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="13">
-        <f>F16+F17</f>
-        <v>8238</v>
+      <c r="C18" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="3">
+        <v>7198</v>
+      </c>
+      <c r="E18" s="3">
+        <v>93</v>
+      </c>
+      <c r="F18" s="1">
+        <f>D18+E18</f>
+        <v>7291</v>
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
@@ -795,134 +745,112 @@
       <c r="J18" s="1"/>
     </row>
     <row r="19" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C19" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="1"/>
+      <c r="C19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" s="3">
+        <v>706</v>
+      </c>
+      <c r="E19" s="3">
+        <v>241</v>
+      </c>
+      <c r="F19" s="1">
+        <f>D19+E19</f>
+        <v>947</v>
+      </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
     </row>
     <row r="20" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="13">
+        <f>F18+F19</f>
+        <v>8238</v>
+      </c>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
     </row>
     <row r="21" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C21" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
+      <c r="C21" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
-      <c r="H21" t="s">
-        <v>14</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="3:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="C22" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>2</v>
-      </c>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+    </row>
+    <row r="22" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
-      <c r="H22" s="10">
-        <v>9280</v>
-      </c>
-      <c r="I22" s="1">
-        <v>4640</v>
-      </c>
-      <c r="J22" s="1">
-        <v>4640</v>
-      </c>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
     </row>
     <row r="23" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C23" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
+      <c r="C23" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
       <c r="F23" s="1"/>
-      <c r="G23" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="H23" s="12">
-        <f>H22*0.2</f>
-        <v>1856</v>
-      </c>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
     </row>
     <row r="24" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C24" s="7" t="s">
+      <c r="C24" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D24" s="7">
-        <v>750</v>
-      </c>
-      <c r="E24" s="7">
-        <v>161</v>
-      </c>
-      <c r="F24" s="1">
-        <f>D24+E24</f>
-        <v>911</v>
-      </c>
-      <c r="G24" s="11">
-        <v>0.8</v>
-      </c>
-      <c r="H24" s="1">
-        <f>H22*0.8</f>
-        <v>7424</v>
-      </c>
+      <c r="E24" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
     </row>
     <row r="25" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C25" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D25" s="7">
-        <v>316</v>
-      </c>
-      <c r="E25" s="7">
-        <v>629</v>
-      </c>
-      <c r="F25" s="1">
-        <f>D25+E25</f>
-        <v>945</v>
-      </c>
+      <c r="C25" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
     </row>
     <row r="26" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="12">
-        <f>F24+F25</f>
-        <v>1856</v>
+      <c r="C26" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26" s="5">
+        <v>7204</v>
+      </c>
+      <c r="E26" s="5">
+        <v>106</v>
+      </c>
+      <c r="F26" s="1">
+        <f>D26+E26</f>
+        <v>7310</v>
       </c>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
@@ -930,33 +858,43 @@
       <c r="J26" s="1"/>
     </row>
     <row r="27" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C27" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="1"/>
+      <c r="C27" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D27" s="5">
+        <v>726</v>
+      </c>
+      <c r="E27" s="5">
+        <v>202</v>
+      </c>
+      <c r="F27" s="1">
+        <f>D27+E27</f>
+        <v>928</v>
+      </c>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
     </row>
     <row r="28" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="13">
+        <f>F26+F27</f>
+        <v>8238</v>
+      </c>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
     </row>
     <row r="29" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C29" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
+      <c r="C29" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
@@ -964,15 +902,9 @@
       <c r="J29" s="1"/>
     </row>
     <row r="30" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C30" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="E30" s="9" t="s">
-        <v>2</v>
-      </c>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
@@ -980,85 +912,113 @@
       <c r="J30" s="1"/>
     </row>
     <row r="31" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C31" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
+      <c r="C31" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
-    </row>
-    <row r="32" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C32" s="9" t="s">
+      <c r="H31" t="s">
+        <v>14</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="3:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="C32" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D32" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D32" s="9">
-        <v>6598</v>
-      </c>
-      <c r="E32" s="9">
-        <v>712</v>
-      </c>
-      <c r="F32" s="1">
-        <f>D32+E32</f>
-        <v>7310</v>
-      </c>
+      <c r="E32" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F32" s="1"/>
       <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
+      <c r="H32" s="10">
+        <v>9280</v>
+      </c>
+      <c r="I32" s="1">
+        <v>4640</v>
+      </c>
+      <c r="J32" s="1">
+        <v>4640</v>
+      </c>
     </row>
     <row r="33" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C33" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D33" s="9">
-        <v>613</v>
-      </c>
-      <c r="E33" s="9">
-        <v>315</v>
-      </c>
-      <c r="F33" s="1">
-        <f>D33+E33</f>
-        <v>928</v>
-      </c>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
+      <c r="C33" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="H33" s="12">
+        <f>H32*0.2</f>
+        <v>1856</v>
+      </c>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
     </row>
     <row r="34" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="13">
-        <f>F32+F33</f>
-        <v>8238</v>
-      </c>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
+      <c r="C34" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D34" s="7">
+        <v>750</v>
+      </c>
+      <c r="E34" s="7">
+        <v>161</v>
+      </c>
+      <c r="F34" s="1">
+        <f>D34+E34</f>
+        <v>911</v>
+      </c>
+      <c r="G34" s="11">
+        <v>0.8</v>
+      </c>
+      <c r="H34" s="1">
+        <f>H32*0.8</f>
+        <v>7424</v>
+      </c>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
     </row>
     <row r="35" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C35" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="1"/>
+      <c r="C35" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D35" s="7">
+        <v>316</v>
+      </c>
+      <c r="E35" s="7">
+        <v>629</v>
+      </c>
+      <c r="F35" s="1">
+        <f>D35+E35</f>
+        <v>945</v>
+      </c>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
     </row>
     <row r="36" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="12">
+        <f>F34+F35</f>
+        <v>1856</v>
+      </c>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
@@ -1066,7 +1026,7 @@
     </row>
     <row r="37" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C37" s="7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
@@ -1077,15 +1037,9 @@
       <c r="J37" s="1"/>
     </row>
     <row r="38" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C38" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D38" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E38" s="7" t="s">
-        <v>2</v>
-      </c>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
@@ -1093,67 +1047,58 @@
       <c r="J38" s="1"/>
     </row>
     <row r="39" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C39" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D39" s="7"/>
-      <c r="E39" s="7"/>
+      <c r="C39" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
       <c r="F39" s="1"/>
-      <c r="G39" s="11">
-        <v>0.3</v>
-      </c>
-      <c r="H39" s="1">
-        <f>F2*0.3</f>
-        <v>12356.4</v>
-      </c>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
     </row>
     <row r="40" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C40" s="7" t="s">
+      <c r="C40" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D40" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D40" s="7">
-        <v>8411</v>
-      </c>
-      <c r="E40" s="7">
-        <v>2554</v>
-      </c>
-      <c r="F40" s="1">
-        <f>D40+E40</f>
-        <v>10965</v>
-      </c>
+      <c r="E40" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F40" s="1"/>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
     </row>
     <row r="41" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C41" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D41" s="7">
-        <v>454</v>
-      </c>
-      <c r="E41" s="7">
-        <v>938</v>
-      </c>
-      <c r="F41" s="1">
-        <f>D41+E41</f>
-        <v>1392</v>
-      </c>
+      <c r="C41" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="1"/>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
     </row>
     <row r="42" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C42" s="7"/>
-      <c r="D42" s="7"/>
-      <c r="E42" s="7"/>
+      <c r="C42" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D42" s="9">
+        <v>6598</v>
+      </c>
+      <c r="E42" s="9">
+        <v>712</v>
+      </c>
       <c r="F42" s="1">
-        <f>F40+F41</f>
-        <v>12357</v>
+        <f>D42+E42</f>
+        <v>7310</v>
       </c>
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
@@ -1161,18 +1106,171 @@
       <c r="J42" s="1"/>
     </row>
     <row r="43" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C43" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D43" s="7"/>
-      <c r="E43" s="7"/>
-      <c r="F43" s="1"/>
+      <c r="C43" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D43" s="9">
+        <v>613</v>
+      </c>
+      <c r="E43" s="9">
+        <v>315</v>
+      </c>
+      <c r="F43" s="1">
+        <f>D43+E43</f>
+        <v>928</v>
+      </c>
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
     </row>
+    <row r="44" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C44" s="9"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="9"/>
+      <c r="F44" s="13">
+        <f>F42+F43</f>
+        <v>8238</v>
+      </c>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
+      <c r="J44" s="1"/>
+    </row>
+    <row r="45" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C45" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D45" s="9"/>
+      <c r="E45" s="9"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
+      <c r="J45" s="1"/>
+    </row>
+    <row r="46" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
+      <c r="J46" s="1"/>
+    </row>
+    <row r="47" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C47" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
+      <c r="I47" s="1"/>
+      <c r="J47" s="1"/>
+    </row>
+    <row r="48" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C48" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E48" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+      <c r="H48" s="1"/>
+      <c r="I48" s="1"/>
+      <c r="J48" s="1"/>
+    </row>
+    <row r="49" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C49" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D49" s="7"/>
+      <c r="E49" s="7"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="11">
+        <v>0.3</v>
+      </c>
+      <c r="H49" s="1">
+        <f>F12*0.3</f>
+        <v>12356.4</v>
+      </c>
+      <c r="I49" s="1"/>
+      <c r="J49" s="1"/>
+    </row>
+    <row r="50" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C50" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D50" s="7">
+        <v>8411</v>
+      </c>
+      <c r="E50" s="7">
+        <v>2554</v>
+      </c>
+      <c r="F50" s="1">
+        <f>D50+E50</f>
+        <v>10965</v>
+      </c>
+      <c r="G50" s="1"/>
+      <c r="H50" s="1"/>
+      <c r="I50" s="1"/>
+      <c r="J50" s="1"/>
+    </row>
+    <row r="51" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C51" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D51" s="7">
+        <v>454</v>
+      </c>
+      <c r="E51" s="7">
+        <v>938</v>
+      </c>
+      <c r="F51" s="1">
+        <f>D51+E51</f>
+        <v>1392</v>
+      </c>
+      <c r="G51" s="1"/>
+      <c r="H51" s="1"/>
+      <c r="I51" s="1"/>
+      <c r="J51" s="1"/>
+    </row>
+    <row r="52" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C52" s="7"/>
+      <c r="D52" s="7"/>
+      <c r="E52" s="7"/>
+      <c r="F52" s="1">
+        <f>F50+F51</f>
+        <v>12357</v>
+      </c>
+      <c r="G52" s="1"/>
+      <c r="H52" s="1"/>
+      <c r="I52" s="1"/>
+      <c r="J52" s="1"/>
+    </row>
+    <row r="53" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C53" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D53" s="7"/>
+      <c r="E53" s="7"/>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
+      <c r="H53" s="1"/>
+      <c r="I53" s="1"/>
+      <c r="J53" s="1"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C2:J9"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>